<commit_message>
SE-341 Register handlers in the service.properties.
SVN: 21607
</commit_message>
<xml_diff>
--- a/eu_basynthec/sourceTest/examples/Proteomics-BadHeader.xlsx
+++ b/eu_basynthec/sourceTest/examples/Proteomics-BadHeader.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6240" yWindow="5820" windowWidth="23400" windowHeight="16220" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="6240" yWindow="5820" windowWidth="23400" windowHeight="16220" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="openbis-metadata" sheetId="1" r:id="rId1"/>
@@ -553,7 +553,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
@@ -657,7 +657,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>

</xml_diff>